<commit_message>
Added the updated Excel file and working on the presentation
</commit_message>
<xml_diff>
--- a/Beaglebone_IoT_activity.xlsx
+++ b/Beaglebone_IoT_activity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ISQA Subjects\Dr. Pawaskar work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EACEF45-2216-4FB5-BE92-955C0A92AC23}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83B558E-5444-48A3-A42B-B154C53F8824}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{61EF915C-E332-4B05-8936-31D72E39F4BF}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
   <si>
     <t>Serial Number</t>
   </si>
@@ -83,9 +83,6 @@
     <t>https://www.amazon.com/SparkFun-5030-XBEE-Explorer-USB/dp/B008O92TZS/ref=sr_1_1?s=industrial&amp;ie=UTF8&amp;qid=1536862945&amp;sr=1-1&amp;keywords=xbee+dongle&amp;dpID=51P0RYOrvQL&amp;preST=_SX342_QL70_&amp;dpSrc=srch</t>
   </si>
   <si>
-    <t>Xbee Wire Antenna</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/XBee-2mW-Wire-Antenna-ZigBee/dp/B007R9U1QA/ref=sr_1_2?s=electronics&amp;ie=UTF8&amp;qid=1536863104&amp;sr=1-2&amp;keywords=xbee+antenna</t>
   </si>
   <si>
@@ -108,6 +105,15 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>PROJECT COST WITHOUT XBEE DONGLE AND ANTENNA</t>
+  </si>
+  <si>
+    <t>PROJECT COST WITH XBEE DONGLE AND ANTENNA</t>
+  </si>
+  <si>
+    <t>Xbee Antenna</t>
   </si>
 </sst>
 </file>
@@ -504,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DBFDE3D-B1A2-4B72-88CC-3CE80FCCA519}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,61 +525,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1">
-        <v>69.94</v>
-      </c>
-      <c r="G2" s="1">
-        <f>E2*F2</f>
-        <v>69.94</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
@@ -582,22 +569,22 @@
         <v>1</v>
       </c>
       <c r="F3" s="1">
-        <v>5.38</v>
+        <v>69.94</v>
       </c>
       <c r="G3" s="1">
         <f>E3*F3</f>
-        <v>5.38</v>
+        <v>69.94</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
@@ -606,22 +593,22 @@
         <v>1</v>
       </c>
       <c r="F4" s="1">
-        <v>9.99</v>
+        <v>5.38</v>
       </c>
       <c r="G4" s="1">
         <f>E4*F4</f>
-        <v>9.99</v>
+        <v>5.38</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
@@ -630,16 +617,16 @@
         <v>1</v>
       </c>
       <c r="F5" s="1">
-        <v>24.95</v>
+        <v>9.99</v>
       </c>
       <c r="G5" s="1">
         <f>E5*F5</f>
-        <v>24.95</v>
+        <v>9.99</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
@@ -657,16 +644,16 @@
         <v>7.77</v>
       </c>
       <c r="G6" s="1">
-        <f>E6*F6</f>
+        <f t="shared" ref="G6:G8" si="0">E6*F6</f>
         <v>7.77</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>18</v>
@@ -678,82 +665,285 @@
         <v>1</v>
       </c>
       <c r="F7" s="1">
-        <v>26.95</v>
+        <v>5.75</v>
       </c>
       <c r="G7" s="1">
-        <f>E7*F7</f>
-        <v>26.95</v>
+        <f t="shared" si="0"/>
+        <v>5.75</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="1">
+        <f>SUM(G3:G8)</f>
+        <v>99.829999999999984</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1">
+        <v>69.94</v>
+      </c>
+      <c r="G14" s="1">
+        <f>E14*F14</f>
+        <v>69.94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="1">
+        <v>5.38</v>
+      </c>
+      <c r="G15" s="1">
+        <f>E15*F15</f>
+        <v>5.38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>9.99</v>
+      </c>
+      <c r="G16" s="1">
+        <f t="shared" ref="G16:G19" si="1">E16*F16</f>
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>7.77</v>
+      </c>
+      <c r="G17" s="1">
+        <f t="shared" si="1"/>
+        <v>7.77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="C18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
         <v>5.75</v>
       </c>
-      <c r="G8" s="1">
-        <f>E8*F8</f>
+      <c r="G18" s="1">
+        <f t="shared" si="1"/>
         <v>5.75</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>24.95</v>
+      </c>
+      <c r="G20" s="1">
+        <f>E20*F20</f>
+        <v>24.95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21" s="3">
+        <v>26.95</v>
+      </c>
+      <c r="G21" s="1">
+        <f>E21*F21</f>
+        <v>26.95</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
         <v>24</v>
       </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="3">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1">
-        <f>E9*F9</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G12" s="1">
-        <f>SUM(G2:G9)</f>
+      <c r="G23" s="1">
+        <f>SUM(G14:G21)</f>
         <v>151.72999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{3D3E5872-166E-4D80-8E4C-A6BFA30E87BE}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{DFE972F8-31CF-4352-B7C4-3EB68276E888}"/>
-    <hyperlink ref="C6" r:id="rId4" xr:uid="{03A5FC1F-4468-464D-96B1-BAB293A75F8E}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{430E1BCC-2BA2-4B51-BBE9-12A8348C894C}"/>
-    <hyperlink ref="C7" r:id="rId6" xr:uid="{C6E61DA8-C9D4-4B50-AB1A-BBCE6B066EE7}"/>
-    <hyperlink ref="C8" r:id="rId7" xr:uid="{EA1DE737-CFFD-49F4-9384-CEDF4E900211}"/>
-    <hyperlink ref="C9" r:id="rId8" xr:uid="{74FFC01C-FF1A-43F4-AE80-8556D69B7C6D}"/>
+    <hyperlink ref="C5" r:id="rId1" xr:uid="{9A81E1DD-465D-41D6-8898-C553AD2A980E}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{75122A64-265A-4DE1-BED5-2471C3A4B054}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{D5F52274-314B-49B2-9B8D-D846F6AB84EF}"/>
+    <hyperlink ref="C6" r:id="rId4" xr:uid="{6FDA707C-E091-4350-A467-6986AC6BB594}"/>
+    <hyperlink ref="C7" r:id="rId5" xr:uid="{798BB404-2047-4700-A317-B694B72989F1}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{012FC4C5-6113-4DE8-8718-8F256288270F}"/>
+    <hyperlink ref="C20" r:id="rId7" xr:uid="{C79D1524-A4FA-4B57-B232-0ADC112E4DA0}"/>
+    <hyperlink ref="C21" r:id="rId8" xr:uid="{7D781499-6BE4-4E8B-B847-7E8AC18991CA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>